<commit_message>
Correction des fautes d’orthographe
et ajout des accents
</commit_message>
<xml_diff>
--- a/LIVRABLE-1/Gestion de projet/Analyse des risques.xlsx
+++ b/LIVRABLE-1/Gestion de projet/Analyse des risques.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentin/Documents/CESI COURS/PFR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain.CHRETIEN\Documents\CESI\snir-co\LIVRABLE-1\Gestion de projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D849E2B-9DD4-DA41-9503-92EBFE70BB26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A452EF0E-BA11-4583-9D41-9FD06B76BC41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16200" xr2:uid="{AEB1E3CF-BFBB-E542-BB1C-6ABE6305FB4E}"/>
+    <workbookView xWindow="384" yWindow="456" windowWidth="28044" windowHeight="16200" xr2:uid="{AEB1E3CF-BFBB-E542-BB1C-6ABE6305FB4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -51,9 +50,6 @@
     <t>Le client n'est pas disponible durant le projet</t>
   </si>
   <si>
-    <t>Planifier des rendez vous avec le client</t>
-  </si>
-  <si>
     <t>Communication au sein de l'équipe</t>
   </si>
   <si>
@@ -66,21 +62,12 @@
     <t>Equipe</t>
   </si>
   <si>
-    <t>Toujours etre en contact sur l'évolution et echanger au sein de l'équipe</t>
-  </si>
-  <si>
     <t>Gestion du planning</t>
   </si>
   <si>
-    <t>Chaque membre doit etre assidus et répondre au planning mis en place</t>
-  </si>
-  <si>
     <t>Rendus des documents</t>
   </si>
   <si>
-    <t>Les documents doivent etre prêt a temps et complets</t>
-  </si>
-  <si>
     <t>Projet</t>
   </si>
   <si>
@@ -99,21 +86,9 @@
     <t>Connaissance du projet</t>
   </si>
   <si>
-    <t xml:space="preserve">Un code robuste sera plus simple a faire evoluer </t>
-  </si>
-  <si>
-    <t>Le formats de données devra etre choisis par l'équipe</t>
-  </si>
-  <si>
     <t>Une solution simple d'utilisation et agréable pour le client</t>
   </si>
   <si>
-    <t>Le projet devra etre fait dans des technologies connus par le groupe pour eviter la perte de temps d'apprentissage</t>
-  </si>
-  <si>
-    <t>Le projet devra etre bien compris pour rendre quelque chose de complet en adéquation avec la demande client</t>
-  </si>
-  <si>
     <t>Compréhension du métier client</t>
   </si>
   <si>
@@ -123,18 +98,9 @@
     <t>Principe de devis</t>
   </si>
   <si>
-    <t>Connaitre les differents point que comporteront les devis</t>
-  </si>
-  <si>
     <t>Sauvegarde locale et/ou cloud</t>
   </si>
   <si>
-    <t>Mise au point sur les differents moyens de sauvegarde</t>
-  </si>
-  <si>
-    <t>Mise au point avec le client sur le besoin d'etre en ligne ou hors ligne</t>
-  </si>
-  <si>
     <t>Utilisation de la solution en ligne ou hors ligne</t>
   </si>
   <si>
@@ -150,13 +116,46 @@
     <t>Possibilité de réduction</t>
   </si>
   <si>
-    <t>Des réductions devront pouvoir etre appliquées aux devis</t>
-  </si>
-  <si>
     <t>Respect de la séparation des taches</t>
   </si>
   <si>
     <t>Chacun devra faire sa partie du travail tout en étant si possible disponible pour aider autrui</t>
+  </si>
+  <si>
+    <t>Planifier des rendez-vous avec le client</t>
+  </si>
+  <si>
+    <t>Toujours être en contact sur l'évolution et échanger au sein de l'équipe</t>
+  </si>
+  <si>
+    <t>Les documents doivent être prêt à temps et complets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un code robuste sera plus simple a faire évoluer </t>
+  </si>
+  <si>
+    <t>Le formats de données devra être choisis par l'équipe</t>
+  </si>
+  <si>
+    <t>Chaque membres doit être assidus et répondrent au planning mis en place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nous devrons utiliser chacunes des compétences technologiques présentent au sein de l'équipe </t>
+  </si>
+  <si>
+    <t>Le projet devra être bien compris pour rendre quelque chose de complet en adéquation avec la demande client</t>
+  </si>
+  <si>
+    <t>Connaître les différents point que comporteront les devis</t>
+  </si>
+  <si>
+    <t>Mise au point sur les différents moyens de sauvegarde</t>
+  </si>
+  <si>
+    <t>Mise au point avec le client sur le besoin d'être en ligne ou hors ligne</t>
+  </si>
+  <si>
+    <t>Des réductions devront pouvoir être appliquées aux devis</t>
   </si>
 </sst>
 </file>
@@ -349,15 +348,6 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -397,6 +387,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,193 +713,193 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.83203125" customWidth="1"/>
-    <col min="2" max="2" width="42.1640625" customWidth="1"/>
+    <col min="1" max="1" width="42.796875" customWidth="1"/>
+    <col min="2" max="2" width="42.19921875" customWidth="1"/>
     <col min="3" max="3" width="98" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="21" t="s">
+      <c r="B5" s="17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="C5" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="21" t="s">
+      <c r="C6" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="20" t="s">
+      <c r="C7" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="20" t="s">
+      <c r="C9" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C10" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="20" t="s">
+      <c r="C11" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="21" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
-      <c r="B15" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
-      <c r="B16" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
-      <c r="B19" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>